<commit_message>
Auto update md files
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -94,7 +94,7 @@
     <t>中</t>
   </si>
   <si>
-    <t>进行中</t>
+    <t>未完成</t>
   </si>
   <si>
     <r>
@@ -132,6 +132,9 @@
     <t>低</t>
   </si>
   <si>
+    <t>进行中</t>
+  </si>
+  <si>
     <t>已经在线提交了</t>
   </si>
   <si>
@@ -185,9 +188,6 @@
   </si>
   <si>
     <t>超市采购生活用品</t>
-  </si>
-  <si>
-    <t>未完成</t>
   </si>
   <si>
     <t>记得买鸡蛋和牛奶</t>
@@ -923,7 +923,7 @@
     <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="25">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -970,13 +970,6 @@
       <fill>
         <patternFill patternType="solid">
           <bgColor theme="6" tint="0.8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1180,25 +1173,25 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
     <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{59DB682C-5494-4EDE-A608-00C9E5F0F923}">
-      <tableStyleElement type="wholeTable" dxfId="15"/>
-      <tableStyleElement type="headerRow" dxfId="14"/>
-      <tableStyleElement type="totalRow" dxfId="13"/>
-      <tableStyleElement type="firstColumn" dxfId="12"/>
-      <tableStyleElement type="lastColumn" dxfId="11"/>
-      <tableStyleElement type="firstRowStripe" dxfId="10"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="9"/>
+      <tableStyleElement type="wholeTable" dxfId="14"/>
+      <tableStyleElement type="headerRow" dxfId="13"/>
+      <tableStyleElement type="totalRow" dxfId="12"/>
+      <tableStyleElement type="firstColumn" dxfId="11"/>
+      <tableStyleElement type="lastColumn" dxfId="10"/>
+      <tableStyleElement type="firstRowStripe" dxfId="9"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="8"/>
     </tableStyle>
     <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{267968C8-6FFD-4C36-ACC1-9EA1FD1885CA}">
-      <tableStyleElement type="headerRow" dxfId="25"/>
-      <tableStyleElement type="totalRow" dxfId="24"/>
-      <tableStyleElement type="firstRowStripe" dxfId="23"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="22"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="21"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="20"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="19"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="18"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="17"/>
-      <tableStyleElement type="pageFieldValues" dxfId="16"/>
+      <tableStyleElement type="headerRow" dxfId="24"/>
+      <tableStyleElement type="totalRow" dxfId="23"/>
+      <tableStyleElement type="firstRowStripe" dxfId="22"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="21"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="20"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="19"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="18"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="17"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="16"/>
+      <tableStyleElement type="pageFieldValues" dxfId="15"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1462,7 +1455,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="13.5" outlineLevelRow="6" outlineLevelCol="6"/>
@@ -1543,7 +1536,7 @@
       </c>
       <c r="G3" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
-        <v>进行中</v>
+        <v>未完成</v>
       </c>
     </row>
     <row r="4" ht="16.5" spans="1:7">
@@ -1558,22 +1551,22 @@
         <v>16</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G4" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
-        <v>已完成</v>
+        <v>已逾期</v>
       </c>
     </row>
     <row r="5" ht="31.5" spans="1:7">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="3">
-        <v>46045</v>
+        <v>46051</v>
       </c>
       <c r="C5" s="4">
         <v>0.625</v>
@@ -1585,19 +1578,19 @@
         <v>13</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G5" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
-        <v>已逾期</v>
+        <v>未完成</v>
       </c>
     </row>
     <row r="6" ht="16.5" spans="1:7">
       <c r="A6" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" s="3">
-        <v>46047</v>
+        <v>46050</v>
       </c>
       <c r="C6" s="4">
         <v>0.770833333333333</v>
@@ -1606,14 +1599,14 @@
         <v>12</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>22</v>
       </c>
       <c r="G6" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
-        <v>已逾期</v>
+        <v>已完成</v>
       </c>
     </row>
     <row r="7" ht="16.5" spans="1:7">
@@ -1628,7 +1621,7 @@
         <v>16</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>24</v>
@@ -1688,7 +1681,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G1048576">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>$G2="已逾期"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>